<commit_message>
Reran marking on Assignment 1
</commit_message>
<xml_diff>
--- a/S2022_Tests/ASS_01_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
+++ b/S2022_Tests/ASS_01_Dim_Testing/StudentFolder/Ex.1/ExcelExtract.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK\S2022_Tests\ASS_01_Dim_Testing\StudentFolder\Ex.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_01_Dim_Testing\StudentFolder\Ex.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{363A00A2-9F68-4744-A119-05AB039DEB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACB96DD4-8C24-4093-9092-0E04F08E6089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{80A376BA-C655-4AB8-9D49-11411578016D}"/>
+    <workbookView xWindow="953" yWindow="2847" windowWidth="13120" windowHeight="7660" xr2:uid="{40F0EB1B-6F86-4D07-9C2A-A46204171294}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
     <t xml:space="preserve"> DSN</t>
   </si>
   <si>
-    <t>C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK\S2022_Tests\ASS_01_Dim_Testing\StudentFolder\Ex.1\Student\MecE265_Ass01_dnobes.SLDPRT</t>
+    <t>C:\Users\zacha\OneDrive\Desktop\Ualberta Summer 2022 Co-op\SolidWorks\AutoMARK\AutoMARK_V6\S2022_Tests\ASS_01_Dim_Testing\StudentFolder\Ex.1\Student\MecE265_Ass01_dnobes.SLDPRT</t>
   </si>
   <si>
     <t>dnobes</t>
@@ -1393,7 +1393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E5F160-A23F-4D11-8104-F972F67D0BFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB35B6C-EB60-4400-8A66-CF85339D9420}">
   <dimension ref="A1:AS125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6725,16 +6725,16 @@
         <v>0</v>
       </c>
       <c r="AP75">
-        <v>0.12144631505565791</v>
+        <v>0.12144631505565784</v>
       </c>
       <c r="AQ75">
-        <v>0.11759504957344208</v>
+        <v>0.11759504957344211</v>
       </c>
       <c r="AR75">
-        <v>0.1444214264313505</v>
+        <v>0.14442142643135047</v>
       </c>
       <c r="AS75">
-        <v>0.1412835332158055</v>
+        <v>0.14128353321580553</v>
       </c>
     </row>
     <row r="76" spans="1:45" x14ac:dyDescent="0.5">
@@ -6841,13 +6841,13 @@
         <v>7.6683870743504176E-2</v>
       </c>
       <c r="AQ76">
-        <v>5.4939291394623724E-2</v>
+        <v>5.4939291394623807E-2</v>
       </c>
       <c r="AR76">
         <v>0.18918387074350418</v>
       </c>
       <c r="AS76">
-        <v>5.4939291394623724E-2</v>
+        <v>5.4939291394623807E-2</v>
       </c>
     </row>
     <row r="77" spans="1:45" x14ac:dyDescent="0.5">
@@ -6951,13 +6951,13 @@
         <v>0</v>
       </c>
       <c r="AP77">
-        <v>6.0683870743504204E-2</v>
+        <v>6.0683870743504176E-2</v>
       </c>
       <c r="AQ77">
         <v>7.6939291394623799E-2</v>
       </c>
       <c r="AR77">
-        <v>6.0683870743504204E-2</v>
+        <v>6.0683870743504176E-2</v>
       </c>
       <c r="AS77">
         <v>9.9439291394623791E-2</v>
@@ -7070,16 +7070,16 @@
         <v>0</v>
       </c>
       <c r="AP78">
-        <v>0.14267665653607917</v>
+        <v>0.14267665653607911</v>
       </c>
       <c r="AQ78">
-        <v>0.12381429139462383</v>
+        <v>0.12381429139462387</v>
       </c>
       <c r="AR78">
-        <v>0.12319108495092926</v>
+        <v>0.1231910849509292</v>
       </c>
       <c r="AS78">
-        <v>0.13506429139462375</v>
+        <v>0.13506429139462378</v>
       </c>
     </row>
     <row r="79" spans="1:45" x14ac:dyDescent="0.5">
@@ -7189,16 +7189,16 @@
         <v>0</v>
       </c>
       <c r="AP79">
-        <v>0.13717651143062351</v>
+        <v>0.13717651143062345</v>
       </c>
       <c r="AQ79">
-        <v>0.12519665070750452</v>
+        <v>0.12519665070750455</v>
       </c>
       <c r="AR79">
-        <v>0.12869123005638491</v>
+        <v>0.12869123005638486</v>
       </c>
       <c r="AS79">
-        <v>0.13368193208174306</v>
+        <v>0.13368193208174309</v>
       </c>
     </row>
     <row r="80" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -8087,13 +8087,13 @@
         <v>0</v>
       </c>
       <c r="AP93">
-        <v>0.21718387074350426</v>
+        <v>0.21718387074350418</v>
       </c>
       <c r="AQ93">
         <v>0.25008438630216817</v>
       </c>
       <c r="AR93">
-        <v>0.21718387074350426</v>
+        <v>0.21718387074350418</v>
       </c>
       <c r="AS93">
         <v>0.17508438630216819</v>
@@ -8212,16 +8212,16 @@
         <v>0</v>
       </c>
       <c r="AP94">
-        <v>0.10338437296230189</v>
+        <v>0.10338437296230187</v>
       </c>
       <c r="AQ94">
-        <v>0.18762813630216824</v>
+        <v>0.18762813630216826</v>
       </c>
       <c r="AR94">
-        <v>8.4483368524706462E-2</v>
+        <v>8.4483368524706434E-2</v>
       </c>
       <c r="AS94">
-        <v>0.19854063630216812</v>
+        <v>0.19854063630216814</v>
       </c>
     </row>
     <row r="95" spans="1:45" x14ac:dyDescent="0.5">
@@ -8325,13 +8325,13 @@
         <v>0</v>
       </c>
       <c r="AP95">
-        <v>0.20518387074350419</v>
+        <v>0.20518387074350417</v>
       </c>
       <c r="AQ95">
         <v>0.25008438630216817</v>
       </c>
       <c r="AR95">
-        <v>0.20518387074350419</v>
+        <v>0.20518387074350417</v>
       </c>
       <c r="AS95">
         <v>0.23058438630216818</v>
@@ -8438,13 +8438,13 @@
         <v>0</v>
       </c>
       <c r="AP96">
-        <v>0.20518387074350419</v>
+        <v>0.20518387074350417</v>
       </c>
       <c r="AQ96">
         <v>0.23058438630216818</v>
       </c>
       <c r="AR96">
-        <v>0.20518387074350419</v>
+        <v>0.20518387074350417</v>
       </c>
       <c r="AS96">
         <v>0.19308438630216818</v>
@@ -8554,13 +8554,13 @@
         <v>9.3933870743504178E-2</v>
       </c>
       <c r="AQ97">
-        <v>0.2600843863021679</v>
+        <v>0.26008438630216796</v>
       </c>
       <c r="AR97">
         <v>0.17193387074350416</v>
       </c>
       <c r="AS97">
-        <v>0.2600843863021679</v>
+        <v>0.26008438630216796</v>
       </c>
     </row>
     <row r="98" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -9921,7 +9921,7 @@
         <v>0.30030409764052635</v>
       </c>
       <c r="AQ116">
-        <v>0.1022573665580863</v>
+        <v>0.10225736655808633</v>
       </c>
       <c r="AR116">
         <v>0</v>
@@ -10266,13 +10266,13 @@
         <v>0.28263023505962626</v>
       </c>
       <c r="AQ119">
-        <v>0.16793929139462396</v>
+        <v>0.16793929139462399</v>
       </c>
       <c r="AR119">
         <v>0.31413023505962628</v>
       </c>
       <c r="AS119">
-        <v>0.16793929139462396</v>
+        <v>0.16793929139462399</v>
       </c>
     </row>
     <row r="120" spans="1:45" x14ac:dyDescent="0.5">
@@ -10379,13 +10379,13 @@
         <v>0.2826302350596262</v>
       </c>
       <c r="AQ120">
-        <v>0.16193929139462399</v>
+        <v>0.16193929139462401</v>
       </c>
       <c r="AR120">
         <v>0.29163023505962621</v>
       </c>
       <c r="AS120">
-        <v>0.16193929139462399</v>
+        <v>0.16193929139462401</v>
       </c>
     </row>
     <row r="121" spans="1:45" x14ac:dyDescent="0.5">

</xml_diff>